<commit_message>
arrange widgets & add graph initialization
</commit_message>
<xml_diff>
--- a/durability.xlsx
+++ b/durability.xlsx
@@ -1,40 +1,171 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Measurement_Program\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92545BB9-F5CF-4AC7-9C1A-1C7A440510C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+  <si>
+    <t>start_but</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>stop_but</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSV File Path</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entry</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Browse</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Load CSV</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>V Limit</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Time</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interval</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update Values</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Graph</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bar</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Terminal</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clear Terminal</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Export</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,85 +173,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="5">
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="中等" xfId="3" builtinId="28"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="備註" xfId="4" builtinId="10"/>
+    <cellStyle name="壞" xfId="2" builtinId="27"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,45 +515,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
+    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>